<commit_message>
Additional graphs, minor changes and frozen final model
</commit_message>
<xml_diff>
--- a/Gesture_elicitation/Elicited_gestures.xlsx
+++ b/Gesture_elicitation/Elicited_gestures.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ieva\Documents\Coding\IIB_Project\Gesture_elicitation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13C255B-7E71-420E-83D7-1EFAC5703684}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C315AAA9-9669-4298-BFC8-8E28D8129FBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elicited_gestures" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Elicited_gestures!$A$1:$Y$101</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -399,9 +402,6 @@
     <t>Grab it in a hook like motion (into full thumb) and drag it to one of the sides off the plane</t>
   </si>
   <si>
-    <t>Arbitrary mapping</t>
-  </si>
-  <si>
     <t>A hook movement with 2 fingers to "hook" the object into place</t>
   </si>
   <si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>Gesture comfort</t>
+  </si>
+  <si>
+    <t>Time, s</t>
   </si>
 </sst>
 </file>
@@ -1019,8 +1022,8 @@
   <dimension ref="A1:Y999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1061,7 +1064,9 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3"/>
+      <c r="J1" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1134,7 +1139,9 @@
         <v>2</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="3">
+        <v>50</v>
+      </c>
       <c r="K2" s="9">
         <v>1</v>
       </c>
@@ -1183,7 +1190,9 @@
       <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="3">
+        <v>35</v>
+      </c>
       <c r="K3" s="9">
         <v>1</v>
       </c>
@@ -1234,7 +1243,9 @@
       <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3">
+        <v>10</v>
+      </c>
       <c r="K4" s="9">
         <v>1</v>
       </c>
@@ -1287,7 +1298,9 @@
       <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3">
+        <v>55</v>
+      </c>
       <c r="K5" s="9">
         <v>1</v>
       </c>
@@ -1336,7 +1349,9 @@
         <v>4</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
       <c r="K6" s="9">
         <v>1</v>
       </c>
@@ -1385,7 +1400,9 @@
         <v>4</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
       <c r="K7" s="9">
         <v>1</v>
       </c>
@@ -1434,7 +1451,9 @@
         <v>2</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="3">
+        <v>40</v>
+      </c>
       <c r="K8" s="9">
         <v>1</v>
       </c>
@@ -1481,7 +1500,9 @@
         <v>4</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3">
+        <v>10</v>
+      </c>
       <c r="K9" s="9">
         <v>1</v>
       </c>
@@ -1530,7 +1551,9 @@
         <v>1</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
       <c r="K10" s="9">
         <v>1</v>
       </c>
@@ -1579,7 +1602,9 @@
         <v>2</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3">
+        <v>20</v>
+      </c>
       <c r="K11" s="9">
         <v>1</v>
       </c>
@@ -1628,7 +1653,9 @@
         <v>3</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="J12" s="3">
+        <v>4</v>
+      </c>
       <c r="K12" s="11"/>
       <c r="L12" s="2">
         <v>1</v>
@@ -1677,7 +1704,9 @@
         <v>3</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
       <c r="K13" s="11"/>
       <c r="L13" s="2">
         <v>1</v>
@@ -1726,7 +1755,9 @@
         <v>4</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3">
+        <v>15</v>
+      </c>
       <c r="K14" s="11"/>
       <c r="L14" s="2">
         <v>1</v>
@@ -1775,7 +1806,9 @@
       <c r="I15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3">
+        <v>12</v>
+      </c>
       <c r="K15" s="11"/>
       <c r="L15" s="2">
         <v>1</v>
@@ -1826,7 +1859,9 @@
       <c r="I16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="3"/>
+      <c r="J16" s="3">
+        <v>60</v>
+      </c>
       <c r="K16" s="11"/>
       <c r="L16" s="2">
         <v>1</v>
@@ -1877,7 +1912,9 @@
         <v>1</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="J17" s="3">
+        <v>5</v>
+      </c>
       <c r="K17" s="11"/>
       <c r="L17" s="2">
         <v>1</v>
@@ -1928,7 +1965,9 @@
         <v>2</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="J18" s="3">
+        <v>7</v>
+      </c>
       <c r="K18" s="11"/>
       <c r="L18" s="2">
         <v>1</v>
@@ -1975,7 +2014,9 @@
         <v>5</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="J19" s="3">
+        <v>5</v>
+      </c>
       <c r="K19" s="11"/>
       <c r="L19" s="2">
         <v>1</v>
@@ -2024,7 +2065,9 @@
         <v>3.5</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="J20" s="3">
+        <v>25</v>
+      </c>
       <c r="K20" s="11"/>
       <c r="L20" s="2">
         <v>1</v>
@@ -2073,7 +2116,9 @@
         <v>5</v>
       </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
       <c r="K21" s="11"/>
       <c r="L21" s="2">
         <v>1</v>
@@ -2122,7 +2167,9 @@
         <v>2</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
       <c r="K22" s="11"/>
       <c r="L22" s="2">
         <v>1</v>
@@ -2171,7 +2218,9 @@
         <v>3</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
+      <c r="J23" s="3">
+        <v>20</v>
+      </c>
       <c r="K23" s="11"/>
       <c r="L23" s="2">
         <v>1</v>
@@ -2220,7 +2269,9 @@
         <v>1</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="J24" s="3">
+        <v>30</v>
+      </c>
       <c r="K24" s="11"/>
       <c r="L24" s="2">
         <v>1</v>
@@ -2269,7 +2320,9 @@
         <v>4</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="J25" s="3">
+        <v>5</v>
+      </c>
       <c r="K25" s="11"/>
       <c r="L25" s="3"/>
       <c r="M25" s="2">
@@ -2322,7 +2375,9 @@
         <v>3</v>
       </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="J26" s="3">
+        <v>20</v>
+      </c>
       <c r="K26" s="11"/>
       <c r="L26" s="3"/>
       <c r="M26" s="2">
@@ -2375,7 +2430,9 @@
         <v>2</v>
       </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="J27" s="3">
+        <v>2</v>
+      </c>
       <c r="K27" s="11"/>
       <c r="L27" s="3"/>
       <c r="M27" s="2">
@@ -2428,7 +2485,9 @@
         <v>4</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="J28" s="3">
+        <v>8</v>
+      </c>
       <c r="K28" s="11"/>
       <c r="L28" s="3"/>
       <c r="M28" s="2">
@@ -2481,7 +2540,9 @@
         <v>5</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="J29" s="3">
+        <v>20</v>
+      </c>
       <c r="K29" s="11"/>
       <c r="L29" s="3"/>
       <c r="M29" s="2">
@@ -2536,7 +2597,9 @@
         <v>5</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
       <c r="K30" s="11"/>
       <c r="L30" s="3"/>
       <c r="M30" s="2">
@@ -2591,9 +2654,11 @@
         <v>3</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="J31" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="J31" s="3">
+        <v>2</v>
+      </c>
       <c r="K31" s="11"/>
       <c r="L31" s="3"/>
       <c r="M31" s="2">
@@ -2646,7 +2711,9 @@
         <v>3</v>
       </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="J32" s="3">
+        <v>18</v>
+      </c>
       <c r="K32" s="11"/>
       <c r="L32" s="3"/>
       <c r="M32" s="2">
@@ -2699,7 +2766,9 @@
         <v>3</v>
       </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="J33" s="3">
+        <v>50</v>
+      </c>
       <c r="K33" s="11"/>
       <c r="L33" s="3"/>
       <c r="M33" s="2">
@@ -2752,7 +2821,9 @@
         <v>2</v>
       </c>
       <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="J34" s="3">
+        <v>15</v>
+      </c>
       <c r="K34" s="11"/>
       <c r="L34" s="3"/>
       <c r="M34" s="2">
@@ -2805,7 +2876,9 @@
         <v>4</v>
       </c>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="J35" s="3">
+        <v>10</v>
+      </c>
       <c r="K35" s="11"/>
       <c r="L35" s="3"/>
       <c r="M35" s="2">
@@ -2858,7 +2931,9 @@
         <v>4</v>
       </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="J36" s="3">
+        <v>45</v>
+      </c>
       <c r="K36" s="11"/>
       <c r="L36" s="3"/>
       <c r="M36" s="2">
@@ -2915,7 +2990,9 @@
       <c r="I37" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J37" s="3"/>
+      <c r="J37" s="3">
+        <v>2</v>
+      </c>
       <c r="K37" s="11"/>
       <c r="L37" s="3"/>
       <c r="M37" s="2">
@@ -2970,7 +3047,9 @@
       <c r="I38" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J38" s="3"/>
+      <c r="J38" s="3">
+        <v>30</v>
+      </c>
       <c r="K38" s="11"/>
       <c r="L38" s="3"/>
       <c r="M38" s="2">
@@ -3023,7 +3102,9 @@
         <v>4</v>
       </c>
       <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="3">
+        <v>1</v>
+      </c>
       <c r="K39" s="11"/>
       <c r="L39" s="3"/>
       <c r="M39" s="2">
@@ -3076,7 +3157,9 @@
         <v>4</v>
       </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="3">
+        <v>5</v>
+      </c>
       <c r="K40" s="11"/>
       <c r="L40" s="3"/>
       <c r="M40" s="2">
@@ -3131,7 +3214,9 @@
         <v>3</v>
       </c>
       <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
       <c r="K41" s="11"/>
       <c r="L41" s="3"/>
       <c r="M41" s="2">
@@ -3186,7 +3271,9 @@
         <v>3.5</v>
       </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="J42" s="3">
+        <v>40</v>
+      </c>
       <c r="K42" s="11"/>
       <c r="L42" s="3"/>
       <c r="M42" s="2">
@@ -3241,7 +3328,9 @@
       <c r="I43" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J43" s="3"/>
+      <c r="J43" s="3">
+        <v>5</v>
+      </c>
       <c r="K43" s="11"/>
       <c r="L43" s="3"/>
       <c r="M43" s="2">
@@ -3296,7 +3385,9 @@
         <v>4</v>
       </c>
       <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="J44" s="3">
+        <v>10</v>
+      </c>
       <c r="K44" s="11"/>
       <c r="L44" s="3"/>
       <c r="M44" s="2">
@@ -3353,7 +3444,9 @@
       <c r="I45" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J45" s="3"/>
+      <c r="J45" s="3">
+        <v>1</v>
+      </c>
       <c r="K45" s="11"/>
       <c r="L45" s="3"/>
       <c r="M45" s="2">
@@ -3408,7 +3501,9 @@
       <c r="I46" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3">
+        <v>4</v>
+      </c>
       <c r="K46" s="11"/>
       <c r="L46" s="2">
         <v>1</v>
@@ -3457,7 +3552,9 @@
         <v>4</v>
       </c>
       <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="3">
+        <v>6</v>
+      </c>
       <c r="K47" s="11"/>
       <c r="L47" s="2">
         <v>1</v>
@@ -3508,7 +3605,9 @@
       <c r="I48" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J48" s="3"/>
+      <c r="J48" s="3">
+        <v>4</v>
+      </c>
       <c r="K48" s="11"/>
       <c r="L48" s="3"/>
       <c r="M48" s="2">
@@ -3561,7 +3660,9 @@
         <v>4</v>
       </c>
       <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="J49" s="3">
+        <v>3</v>
+      </c>
       <c r="K49" s="11"/>
       <c r="L49" s="3"/>
       <c r="M49" s="2">
@@ -3616,7 +3717,9 @@
         <v>3.5</v>
       </c>
       <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="J50" s="3">
+        <v>5</v>
+      </c>
       <c r="K50" s="11"/>
       <c r="L50" s="3"/>
       <c r="M50" s="2">
@@ -3671,7 +3774,9 @@
       <c r="I51" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J51" s="3"/>
+      <c r="J51" s="3">
+        <v>2</v>
+      </c>
       <c r="K51" s="11"/>
       <c r="L51" s="3"/>
       <c r="M51" s="2">
@@ -3726,7 +3831,9 @@
         <v>2</v>
       </c>
       <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="J52" s="3">
+        <v>1</v>
+      </c>
       <c r="K52" s="11"/>
       <c r="L52" s="3"/>
       <c r="M52" s="2">
@@ -3779,7 +3886,9 @@
         <v>4</v>
       </c>
       <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="J53" s="3">
+        <v>1</v>
+      </c>
       <c r="K53" s="11"/>
       <c r="L53" s="3"/>
       <c r="M53" s="2">
@@ -3834,7 +3943,9 @@
       <c r="I54" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J54" s="3"/>
+      <c r="J54" s="3">
+        <v>0</v>
+      </c>
       <c r="K54" s="11"/>
       <c r="L54" s="3"/>
       <c r="M54" s="2">
@@ -3891,7 +4002,9 @@
       <c r="I55" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J55" s="3"/>
+      <c r="J55" s="3">
+        <v>3</v>
+      </c>
       <c r="K55" s="11"/>
       <c r="L55" s="3"/>
       <c r="M55" s="2">
@@ -3944,7 +4057,9 @@
         <v>2</v>
       </c>
       <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
+      <c r="J56" s="3">
+        <v>40</v>
+      </c>
       <c r="K56" s="11"/>
       <c r="L56" s="3"/>
       <c r="M56" s="2">
@@ -3999,7 +4114,9 @@
         <v>3</v>
       </c>
       <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
+      <c r="J57" s="3">
+        <v>5</v>
+      </c>
       <c r="K57" s="11"/>
       <c r="L57" s="3"/>
       <c r="M57" s="2">
@@ -4054,7 +4171,9 @@
         <v>5</v>
       </c>
       <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
+      <c r="J58" s="3">
+        <v>7</v>
+      </c>
       <c r="K58" s="11"/>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
@@ -4107,7 +4226,9 @@
         <v>3.5</v>
       </c>
       <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
+      <c r="J59" s="3">
+        <v>45</v>
+      </c>
       <c r="K59" s="11"/>
       <c r="L59" s="3"/>
       <c r="M59" s="2">
@@ -4160,7 +4281,9 @@
         <v>2</v>
       </c>
       <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
+      <c r="J60" s="3">
+        <v>20</v>
+      </c>
       <c r="K60" s="11"/>
       <c r="L60" s="3"/>
       <c r="M60" s="2">
@@ -4213,7 +4336,9 @@
         <v>4</v>
       </c>
       <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
+      <c r="J61" s="3">
+        <v>10</v>
+      </c>
       <c r="K61" s="11"/>
       <c r="L61" s="3"/>
       <c r="M61" s="2">
@@ -4266,7 +4391,9 @@
         <v>3.5</v>
       </c>
       <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
+      <c r="J62" s="3">
+        <v>1</v>
+      </c>
       <c r="K62" s="11"/>
       <c r="L62" s="3"/>
       <c r="M62" s="2">
@@ -4321,7 +4448,9 @@
         <v>3.5</v>
       </c>
       <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
+      <c r="J63" s="3">
+        <v>1</v>
+      </c>
       <c r="K63" s="11"/>
       <c r="L63" s="3"/>
       <c r="M63" s="2">
@@ -4376,7 +4505,9 @@
         <v>2</v>
       </c>
       <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
+      <c r="J64" s="3">
+        <v>3</v>
+      </c>
       <c r="K64" s="11"/>
       <c r="L64" s="3"/>
       <c r="M64" s="2">
@@ -4429,7 +4560,9 @@
         <v>5</v>
       </c>
       <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
+      <c r="J65" s="3">
+        <v>5</v>
+      </c>
       <c r="K65" s="11"/>
       <c r="L65" s="3"/>
       <c r="M65" s="2">
@@ -4482,7 +4615,9 @@
         <v>3</v>
       </c>
       <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
+      <c r="J66" s="3">
+        <v>16</v>
+      </c>
       <c r="K66" s="11"/>
       <c r="L66" s="3"/>
       <c r="M66" s="2">
@@ -4537,7 +4672,9 @@
       <c r="I67" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J67" s="3"/>
+      <c r="J67" s="3">
+        <v>5</v>
+      </c>
       <c r="K67" s="11"/>
       <c r="L67" s="3"/>
       <c r="M67" s="2">
@@ -4592,7 +4729,9 @@
         <v>4</v>
       </c>
       <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
+      <c r="J68" s="3">
+        <v>97</v>
+      </c>
       <c r="K68" s="11"/>
       <c r="L68" s="3"/>
       <c r="M68" s="2">
@@ -4647,7 +4786,9 @@
         <v>3</v>
       </c>
       <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
+      <c r="J69" s="3">
+        <v>26</v>
+      </c>
       <c r="K69" s="11"/>
       <c r="L69" s="3"/>
       <c r="M69" s="2">
@@ -4702,7 +4843,9 @@
         <v>2.5</v>
       </c>
       <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
+      <c r="J70" s="3">
+        <v>10</v>
+      </c>
       <c r="K70" s="11"/>
       <c r="L70" s="3"/>
       <c r="M70" s="2">
@@ -4757,7 +4900,9 @@
         <v>3</v>
       </c>
       <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
+      <c r="J71" s="3">
+        <v>10</v>
+      </c>
       <c r="K71" s="11"/>
       <c r="L71" s="3"/>
       <c r="M71" s="2">
@@ -4812,7 +4957,9 @@
         <v>3</v>
       </c>
       <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
+      <c r="J72" s="3">
+        <v>14</v>
+      </c>
       <c r="K72" s="11"/>
       <c r="L72" s="3"/>
       <c r="M72" s="2">
@@ -4867,7 +5014,9 @@
         <v>3</v>
       </c>
       <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
+      <c r="J73" s="3">
+        <v>2</v>
+      </c>
       <c r="K73" s="11"/>
       <c r="L73" s="3"/>
       <c r="M73" s="2">
@@ -4920,7 +5069,9 @@
         <v>3</v>
       </c>
       <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
+      <c r="J74" s="3">
+        <v>8</v>
+      </c>
       <c r="K74" s="11"/>
       <c r="L74" s="3"/>
       <c r="M74" s="2">
@@ -4973,7 +5124,9 @@
         <v>3.5</v>
       </c>
       <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
+      <c r="J75" s="3">
+        <v>2</v>
+      </c>
       <c r="K75" s="11"/>
       <c r="L75" s="2">
         <v>1</v>
@@ -5022,7 +5175,9 @@
         <v>2.5</v>
       </c>
       <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
+      <c r="J76" s="3">
+        <v>17</v>
+      </c>
       <c r="K76" s="11"/>
       <c r="L76" s="2">
         <v>1</v>
@@ -5073,7 +5228,9 @@
         <v>5</v>
       </c>
       <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
+      <c r="J77" s="3">
+        <v>30</v>
+      </c>
       <c r="K77" s="11"/>
       <c r="L77" s="3"/>
       <c r="M77" s="3"/>
@@ -5130,7 +5287,9 @@
       <c r="I78" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J78" s="3"/>
+      <c r="J78" s="3">
+        <v>10</v>
+      </c>
       <c r="K78" s="11"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
@@ -5185,7 +5344,9 @@
         <v>4.5</v>
       </c>
       <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
+      <c r="J79" s="3">
+        <v>5</v>
+      </c>
       <c r="K79" s="11"/>
       <c r="L79" s="3"/>
       <c r="M79" s="3"/>
@@ -5240,7 +5401,9 @@
         <v>4</v>
       </c>
       <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
+      <c r="J80" s="3">
+        <v>13</v>
+      </c>
       <c r="K80" s="11"/>
       <c r="L80" s="3"/>
       <c r="M80" s="3"/>
@@ -5293,7 +5456,9 @@
         <v>3</v>
       </c>
       <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
+      <c r="J81" s="3">
+        <v>20</v>
+      </c>
       <c r="K81" s="11"/>
       <c r="L81" s="3"/>
       <c r="M81" s="3"/>
@@ -5346,7 +5511,9 @@
         <v>3</v>
       </c>
       <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
+      <c r="J82" s="3">
+        <v>8</v>
+      </c>
       <c r="K82" s="11"/>
       <c r="L82" s="3"/>
       <c r="M82" s="3"/>
@@ -5399,7 +5566,9 @@
         <v>5</v>
       </c>
       <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
+      <c r="J83" s="3">
+        <v>7</v>
+      </c>
       <c r="K83" s="11"/>
       <c r="L83" s="3"/>
       <c r="M83" s="3"/>
@@ -5454,7 +5623,9 @@
         <v>2</v>
       </c>
       <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
+      <c r="J84" s="3">
+        <v>5</v>
+      </c>
       <c r="K84" s="11"/>
       <c r="L84" s="3"/>
       <c r="M84" s="3"/>
@@ -5509,7 +5680,9 @@
         <v>4</v>
       </c>
       <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
+      <c r="J85" s="3">
+        <v>5</v>
+      </c>
       <c r="K85" s="11"/>
       <c r="L85" s="3"/>
       <c r="M85" s="2">
@@ -5562,7 +5735,9 @@
         <v>5</v>
       </c>
       <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
+      <c r="J86" s="3">
+        <v>1</v>
+      </c>
       <c r="K86" s="11"/>
       <c r="L86" s="3"/>
       <c r="M86" s="2">
@@ -5615,7 +5790,9 @@
         <v>3</v>
       </c>
       <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
+      <c r="J87" s="3">
+        <v>0</v>
+      </c>
       <c r="K87" s="11"/>
       <c r="L87" s="3"/>
       <c r="M87" s="2">
@@ -5668,7 +5845,9 @@
         <v>2.5</v>
       </c>
       <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
+      <c r="J88" s="3">
+        <v>17</v>
+      </c>
       <c r="K88" s="11"/>
       <c r="L88" s="3"/>
       <c r="M88" s="2">
@@ -5721,7 +5900,9 @@
         <v>3</v>
       </c>
       <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
+      <c r="J89" s="3">
+        <v>1</v>
+      </c>
       <c r="K89" s="11"/>
       <c r="L89" s="2">
         <v>1</v>
@@ -5772,7 +5953,9 @@
         <v>5</v>
       </c>
       <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
+      <c r="J90" s="3">
+        <v>0</v>
+      </c>
       <c r="K90" s="11"/>
       <c r="L90" s="3"/>
       <c r="M90" s="3"/>
@@ -5829,7 +6012,9 @@
       <c r="I91" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="J91" s="3"/>
+      <c r="J91" s="3">
+        <v>25</v>
+      </c>
       <c r="K91" s="11"/>
       <c r="L91" s="3"/>
       <c r="M91" s="3"/>
@@ -5884,7 +6069,9 @@
         <v>5</v>
       </c>
       <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
+      <c r="J92" s="3">
+        <v>1</v>
+      </c>
       <c r="K92" s="11"/>
       <c r="L92" s="3"/>
       <c r="M92" s="3"/>
@@ -5937,7 +6124,9 @@
         <v>4</v>
       </c>
       <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
+      <c r="J93" s="3">
+        <v>0</v>
+      </c>
       <c r="K93" s="11"/>
       <c r="L93" s="3"/>
       <c r="M93" s="3"/>
@@ -5990,7 +6179,9 @@
         <v>5</v>
       </c>
       <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
+      <c r="J94" s="3">
+        <v>0</v>
+      </c>
       <c r="K94" s="11"/>
       <c r="L94" s="3"/>
       <c r="M94" s="3"/>
@@ -6043,7 +6234,9 @@
         <v>3</v>
       </c>
       <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
+      <c r="J95" s="3">
+        <v>1</v>
+      </c>
       <c r="K95" s="11"/>
       <c r="L95" s="2"/>
       <c r="M95" s="3"/>
@@ -6098,7 +6291,9 @@
         <v>4</v>
       </c>
       <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
+      <c r="J96" s="3">
+        <v>2</v>
+      </c>
       <c r="K96" s="11"/>
       <c r="L96" s="3"/>
       <c r="M96" s="3"/>
@@ -6153,7 +6348,9 @@
       <c r="I97" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J97" s="3"/>
+      <c r="J97" s="3">
+        <v>40</v>
+      </c>
       <c r="K97" s="11"/>
       <c r="L97" s="3"/>
       <c r="M97" s="3"/>
@@ -6206,7 +6403,9 @@
         <v>2</v>
       </c>
       <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
+      <c r="J98" s="3">
+        <v>15</v>
+      </c>
       <c r="K98" s="11"/>
       <c r="L98" s="3"/>
       <c r="M98" s="3"/>
@@ -6259,7 +6458,9 @@
         <v>3</v>
       </c>
       <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
+      <c r="J99" s="3">
+        <v>20</v>
+      </c>
       <c r="K99" s="11"/>
       <c r="L99" s="3"/>
       <c r="M99" s="3"/>
@@ -6311,10 +6512,10 @@
       <c r="H100" s="2">
         <v>2</v>
       </c>
-      <c r="I100" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J100" s="3"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="3">
+        <v>24</v>
+      </c>
       <c r="K100" s="11"/>
       <c r="L100" s="3"/>
       <c r="M100" s="3"/>
@@ -6349,7 +6550,7 @@
         <v>73</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D101" s="2">
         <v>19</v>
@@ -6367,9 +6568,11 @@
         <v>3</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J101" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="J101" s="3">
+        <v>60</v>
+      </c>
       <c r="K101" s="11"/>
       <c r="L101" s="3"/>
       <c r="M101" s="3"/>
@@ -6422,13 +6625,13 @@
     </row>
     <row r="103" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B103" s="1">
         <v>102</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D103" s="2">
         <v>2</v>
@@ -6456,7 +6659,7 @@
     </row>
     <row r="104" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B104" s="1">
         <v>102</v>
@@ -6496,7 +6699,7 @@
     </row>
     <row r="105" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B105" s="1">
         <v>102</v>
@@ -6536,7 +6739,7 @@
     </row>
     <row r="106" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B106" s="1">
         <v>102</v>
@@ -6576,13 +6779,13 @@
     </row>
     <row r="107" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B107" s="1">
         <v>105</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D107" s="2">
         <v>5</v>
@@ -6618,13 +6821,13 @@
     </row>
     <row r="108" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B108" s="1">
         <v>106</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D108" s="2">
         <v>7</v>
@@ -6660,7 +6863,7 @@
     </row>
     <row r="109" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B109" s="1">
         <v>106</v>
@@ -6700,7 +6903,7 @@
     </row>
     <row r="110" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B110" s="1">
         <v>106</v>
@@ -6740,7 +6943,7 @@
     </row>
     <row r="111" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B111" s="1">
         <v>106</v>
@@ -6780,13 +6983,13 @@
     </row>
     <row r="112" spans="1:25" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B112" s="1">
         <v>106</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D112" s="2">
         <v>14</v>
@@ -6804,7 +7007,7 @@
         <v>4</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J112" s="3"/>
       <c r="K112" s="11"/>
@@ -6824,13 +7027,13 @@
     </row>
     <row r="113" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B113" s="1">
         <v>104</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D113" s="2">
         <v>4</v>
@@ -6866,13 +7069,13 @@
     </row>
     <row r="114" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B114" s="1">
         <v>108</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D114" s="2">
         <v>13</v>
@@ -6908,13 +7111,13 @@
     </row>
     <row r="115" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B115" s="1">
         <v>107</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D115" s="2">
         <v>9</v>
@@ -6950,7 +7153,7 @@
     </row>
     <row r="116" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116" s="1">
         <v>107</v>
@@ -6982,7 +7185,7 @@
     </row>
     <row r="117" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B117" s="1">
         <v>107</v>
@@ -7022,7 +7225,7 @@
     </row>
     <row r="118" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B118" s="1">
         <v>107</v>
@@ -7062,13 +7265,13 @@
     </row>
     <row r="119" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B119" s="1">
         <v>101</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D119" s="2">
         <v>1</v>
@@ -7104,7 +7307,7 @@
     </row>
     <row r="120" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B120" s="1">
         <v>101</v>
@@ -7144,13 +7347,13 @@
     </row>
     <row r="121" spans="1:24" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B121" s="1">
         <v>103</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D121" s="2">
         <v>3</v>
@@ -7186,13 +7389,13 @@
     </row>
     <row r="122" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122" s="1">
         <v>109</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D122" s="2">
         <v>17</v>
@@ -7300,7 +7503,7 @@
     </row>
     <row r="126" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C126" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
@@ -7329,7 +7532,7 @@
         <v>31</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3">
@@ -7853,7 +8056,7 @@
     </row>
     <row r="142" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C142" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
@@ -7882,7 +8085,7 @@
     </row>
     <row r="143" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C143" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
@@ -7938,7 +8141,7 @@
         <v>31</v>
       </c>
       <c r="C145" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D145" s="3"/>
       <c r="E145" s="3">
@@ -8297,7 +8500,7 @@
         <v>37</v>
       </c>
       <c r="C156" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E156" s="3">
         <v>3</v>
@@ -8478,7 +8681,7 @@
       </c>
       <c r="B162" s="3"/>
       <c r="C162" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D162" s="3"/>
       <c r="E162" s="3">
@@ -8698,10 +8901,10 @@
     </row>
     <row r="169" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A169" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D169" s="3"/>
       <c r="E169" s="3">
@@ -8739,7 +8942,7 @@
     </row>
     <row r="170" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C170" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D170" s="3"/>
       <c r="E170" s="3">
@@ -8777,7 +8980,7 @@
     </row>
     <row r="171" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C171" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D171" s="3"/>
       <c r="E171" s="3">
@@ -8815,7 +9018,7 @@
     </row>
     <row r="172" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C172" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D172" s="3"/>
       <c r="E172" s="3">
@@ -8880,7 +9083,7 @@
         <v>37</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D174" s="3"/>
       <c r="E174" s="3">
@@ -8918,7 +9121,7 @@
     </row>
     <row r="175" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C175" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D175" s="3"/>
       <c r="E175" s="3">
@@ -8956,7 +9159,7 @@
     </row>
     <row r="176" spans="1:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C176" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D176" s="3"/>
       <c r="E176" s="3">
@@ -8994,7 +9197,7 @@
     </row>
     <row r="177" spans="3:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C177" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D177" s="3"/>
       <c r="E177" s="3">
@@ -9032,7 +9235,7 @@
     </row>
     <row r="178" spans="3:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C178" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D178" s="3"/>
       <c r="E178" s="3">
@@ -9044,7 +9247,7 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="G178" s="3">
-        <f t="shared" ref="F178:H178" si="10">AVERAGE(G163:G165)</f>
+        <f t="shared" ref="G178:H178" si="10">AVERAGE(G163:G165)</f>
         <v>2</v>
       </c>
       <c r="H178" s="3">
@@ -9070,7 +9273,7 @@
     </row>
     <row r="179" spans="3:24" ht="12.75" x14ac:dyDescent="0.35">
       <c r="C179" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D179" s="3"/>
       <c r="E179" s="3">

</xml_diff>